<commit_message>
ajouts graphics et correction
</commit_message>
<xml_diff>
--- a/ToM/compVsMimic_Etude/EtudeFinale/Resultats/JointGain.xlsx
+++ b/ToM/compVsMimic_Etude/EtudeFinale/Resultats/JointGain.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Discolog\ToM\compVsMimic_Etude\EtudeFinale\Resultats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{74077E2E-9BEB-4E0F-BD6F-A00DA1D61A5B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="satPerceptif" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="restaurantsSat" sheetId="3" r:id="rId3"/>
     <sheet name="Resultats" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Bob</t>
   </si>
@@ -31,9 +37,6 @@
   </si>
   <si>
     <t>Kevin</t>
-  </si>
-  <si>
-    <t>User</t>
   </si>
   <si>
     <t>user</t>
@@ -102,19 +105,13 @@
     <t>Compl.</t>
   </si>
   <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>Maximum</t>
+    <t>Comp.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -282,7 +279,634 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Satisfaction Perçu</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-4AAC-48CD-BBDB-647D1C27AFE2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-4AAC-48CD-BBDB-647D1C27AFE2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(perceptifs!$A$6,perceptifs!$C$6,perceptifs!$E$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.72164051114277472</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.74069823800345425</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.67386820718575124</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(perceptifs!$A$6,perceptifs!$C$6,perceptifs!$E$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.72164051114277472</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.74069823800345425</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.67386820718575124</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>perceptifs!$A$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Comp.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Similaire</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Neutre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>perceptifs!$A$12:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5081967213114753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4262295081967213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5081967213114753</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4AAC-48CD-BBDB-647D1C27AFE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Equité perçue</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent6"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltHorz">
+                <a:fgClr>
+                  <a:schemeClr val="accent1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-4AAC-48CD-BBDB-647D1C27AFE2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltHorz">
+                <a:fgClr>
+                  <a:srgbClr val="C00000"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-4AAC-48CD-BBDB-647D1C27AFE2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltHorz">
+                <a:fgClr>
+                  <a:schemeClr val="accent3"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000026-4AAC-48CD-BBDB-647D1C27AFE2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(perceptifs!$B$6,perceptifs!$D$6,perceptifs!$F$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.9504097477007426</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0674007037167828</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.98624418661324253</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(perceptifs!$B$6,perceptifs!$D$6,perceptifs!$F$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.9504097477007426</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0674007037167828</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.98624418661324253</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>perceptifs!$A$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Comp.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Similaire</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Neutre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>perceptifs!$A$13:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.8852459016393444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8360655737704916</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8360655737704916</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4AAC-48CD-BBDB-647D1C27AFE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="777848408"/>
+        <c:axId val="777848736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="777848408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="777848736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="777848736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.5"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Perception du gain commun</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.7777777777777776E-2"/>
+              <c:y val="0.17670494313210849"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="777848408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -390,7 +1014,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3273-4CC3-872B-1D320393AFBD}"/>
             </c:ext>
@@ -412,7 +1036,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="C00000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -474,7 +1098,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3273-4CC3-872B-1D320393AFBD}"/>
             </c:ext>
@@ -558,7 +1182,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3273-4CC3-872B-1D320393AFBD}"/>
             </c:ext>
@@ -574,11 +1198,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="519150080"/>
-        <c:axId val="519178496"/>
+        <c:axId val="685308432"/>
+        <c:axId val="671759136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="519150080"/>
+        <c:axId val="685308432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,7 +1212,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519178496"/>
+        <c:crossAx val="671759136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -596,7 +1220,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519178496"/>
+        <c:axId val="671759136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,6 +1286,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -694,7 +1338,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="519150080"/>
+        <c:crossAx val="685308432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -749,14 +1393,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -788,11 +1432,50 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1335,27 +2018,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>216159</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>13855</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>468630</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>100965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>433873</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>34990</xdr:rowOff>
+      <xdr:colOff>582930</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>100965</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4">
+        <xdr:cNvPr id="4" name="Graphique 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D97D604-5FEE-475E-BFD9-019A0EDEE03E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C943D5-F647-4EDF-8954-29AC15EE576A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1377,694 +2563,44 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.54556</cdr:x>
-      <cdr:y>0.17918</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.7318</cdr:x>
-      <cdr:y>0.26913</cdr:y>
-    </cdr:to>
-    <cdr:grpSp>
-      <cdr:nvGrpSpPr>
-        <cdr:cNvPr id="31" name="Groupe 30">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>216159</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>13855</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>433873</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>34990</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graphique 4">
+          <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5BE0FECC-2BE8-4FC9-91D3-318A289D9891}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D97D604-5FEE-475E-BFD9-019A0EDEE03E}"/>
             </a:ext>
           </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvGrpSpPr/>
-      </cdr:nvGrpSpPr>
-      <cdr:grpSpPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2301289" y="584061"/>
-          <a:ext cx="785600" cy="293205"/>
-          <a:chOff x="2489210" y="971550"/>
-          <a:chExt cx="849779" cy="315149"/>
-        </a:xfrm>
-      </cdr:grpSpPr>
-      <cdr:grpSp>
-        <cdr:nvGrpSpPr>
-          <cdr:cNvPr id="29" name="Groupe 28">
-            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5BB0550-2A69-49EB-8D1F-5610AAD40CA6}"/>
-              </a:ext>
-            </a:extLst>
-          </cdr:cNvPr>
-          <cdr:cNvGrpSpPr/>
-        </cdr:nvGrpSpPr>
-        <cdr:grpSpPr>
-          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:off x="2489210" y="1157272"/>
-            <a:ext cx="849779" cy="129427"/>
-            <a:chOff x="2489210" y="1157273"/>
-            <a:chExt cx="849779" cy="129426"/>
-          </a:xfrm>
-        </cdr:grpSpPr>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="6" name="Connecteur droit 5">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F23F271D-66D5-4B17-AE95-C1D8D6CBBD68}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:off x="2489210" y="1158698"/>
-              <a:ext cx="849779" cy="7957"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="18" name="Connecteur droit 17">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D1AE3F9-7268-4BF3-8EFC-563030086BC0}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-              <a:off x="2490529" y="1157273"/>
-              <a:ext cx="3643" cy="120665"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="20" name="Connecteur droit 19">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67B54A6B-9D56-4F93-9508-7A969FF332D8}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-              <a:off x="3335657" y="1160084"/>
-              <a:ext cx="3205" cy="126615"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-      </cdr:grpSp>
-      <cdr:sp macro="" textlink="">
-        <cdr:nvSpPr>
-          <cdr:cNvPr id="30" name="ZoneTexte 29">
-            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9BF3845-EFA9-4D7C-AAA2-9A8D8D60391D}"/>
-              </a:ext>
-            </a:extLst>
-          </cdr:cNvPr>
-          <cdr:cNvSpPr txBox="1"/>
-        </cdr:nvSpPr>
-        <cdr:spPr>
-          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:off x="2774692" y="971550"/>
-            <a:ext cx="179387" cy="179387"/>
-          </a:xfrm>
-          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </cdr:spPr>
-        <cdr:txBody>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:r>
-              <a:rPr lang="fr-FR" sz="1400" b="1"/>
-              <a:t>*</a:t>
-            </a:r>
-          </a:p>
-        </cdr:txBody>
-      </cdr:sp>
-    </cdr:grpSp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.35347</cdr:x>
-      <cdr:y>0.11285</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.53963</cdr:x>
-      <cdr:y>0.20264</cdr:y>
-    </cdr:to>
-    <cdr:grpSp>
-      <cdr:nvGrpSpPr>
-        <cdr:cNvPr id="32" name="Groupe 31">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CFE4BD15-6B46-4805-95A5-D03517B459A3}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvGrpSpPr/>
-      </cdr:nvGrpSpPr>
-      <cdr:grpSpPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1491012" y="367850"/>
-          <a:ext cx="785263" cy="292682"/>
-          <a:chOff x="0" y="0"/>
-          <a:chExt cx="849366" cy="314607"/>
-        </a:xfrm>
-      </cdr:grpSpPr>
-      <cdr:grpSp>
-        <cdr:nvGrpSpPr>
-          <cdr:cNvPr id="33" name="Groupe 32">
-            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6BFBBCC4-BE14-4843-8CD8-D27815E5C63B}"/>
-              </a:ext>
-            </a:extLst>
-          </cdr:cNvPr>
-          <cdr:cNvGrpSpPr/>
-        </cdr:nvGrpSpPr>
-        <cdr:grpSpPr>
-          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:off x="0" y="185404"/>
-            <a:ext cx="849366" cy="129203"/>
-            <a:chOff x="0" y="185723"/>
-            <a:chExt cx="849779" cy="129426"/>
-          </a:xfrm>
-        </cdr:grpSpPr>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="35" name="Connecteur droit 34">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2FBBC9A7-275C-4F01-A7D5-AE41B541153F}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:off x="0" y="187148"/>
-              <a:ext cx="849779" cy="7957"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="36" name="Connecteur droit 35">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DF2DA73-8B54-43A5-9BB7-EE5C181554A5}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-              <a:off x="1319" y="185723"/>
-              <a:ext cx="3643" cy="120665"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="37" name="Connecteur droit 36">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DA33B84-45EC-41F6-A56D-D7FAABD41AE4}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-              <a:off x="846447" y="188534"/>
-              <a:ext cx="3205" cy="126615"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-      </cdr:grpSp>
-      <cdr:sp macro="" textlink="">
-        <cdr:nvSpPr>
-          <cdr:cNvPr id="34" name="ZoneTexte 3">
-            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0931AD8-D8AB-479C-9A52-2EB433FFC4B9}"/>
-              </a:ext>
-            </a:extLst>
-          </cdr:cNvPr>
-          <cdr:cNvSpPr txBox="1"/>
-        </cdr:nvSpPr>
-        <cdr:spPr>
-          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:off x="285343" y="0"/>
-            <a:ext cx="179300" cy="179078"/>
-          </a:xfrm>
-          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </cdr:spPr>
-        <cdr:txBody>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:lvl1pPr marL="0" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:r>
-              <a:rPr lang="fr-FR" sz="1400" b="1"/>
-              <a:t>*</a:t>
-            </a:r>
-          </a:p>
-        </cdr:txBody>
-      </cdr:sp>
-    </cdr:grpSp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.3548</cdr:x>
-      <cdr:y>0.04609</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.73124</cdr:x>
-      <cdr:y>0.13469</cdr:y>
-    </cdr:to>
-    <cdr:grpSp>
-      <cdr:nvGrpSpPr>
-        <cdr:cNvPr id="38" name="Groupe 37">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4451BA1E-0349-4D3D-9B89-7414559F4C41}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvGrpSpPr/>
-      </cdr:nvGrpSpPr>
-      <cdr:grpSpPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1496622" y="150237"/>
-          <a:ext cx="1587905" cy="288803"/>
-          <a:chOff x="-192" y="6296"/>
-          <a:chExt cx="849558" cy="310414"/>
-        </a:xfrm>
-      </cdr:grpSpPr>
-      <cdr:grpSp>
-        <cdr:nvGrpSpPr>
-          <cdr:cNvPr id="39" name="Groupe 38">
-            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D430C49C-5E21-4CEE-AA13-7836D02B6F84}"/>
-              </a:ext>
-            </a:extLst>
-          </cdr:cNvPr>
-          <cdr:cNvGrpSpPr/>
-        </cdr:nvGrpSpPr>
-        <cdr:grpSpPr>
-          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:off x="-192" y="185085"/>
-            <a:ext cx="849558" cy="131625"/>
-            <a:chOff x="-192" y="185409"/>
-            <a:chExt cx="850384" cy="132083"/>
-          </a:xfrm>
-        </cdr:grpSpPr>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="41" name="Connecteur droit 40">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD291845-8C47-443B-B6AB-340050BA84D7}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:off x="0" y="186837"/>
-              <a:ext cx="850192" cy="7971"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="42" name="Connecteur droit 41">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{26D84641-E4D1-4D6F-A214-F0B0E08C4D04}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-              <a:off x="-192" y="185409"/>
-              <a:ext cx="2013" cy="104999"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-        <cdr:cxnSp macro="">
-          <cdr:nvCxnSpPr>
-            <cdr:cNvPr id="43" name="Connecteur droit 42">
-              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DE11A41-6987-4103-ABCE-44127566B100}"/>
-                </a:ext>
-              </a:extLst>
-            </cdr:cNvPr>
-            <cdr:cNvCxnSpPr/>
-          </cdr:nvCxnSpPr>
-          <cdr:spPr>
-            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-              <a:off x="848655" y="188225"/>
-              <a:ext cx="1410" cy="129267"/>
-            </a:xfrm>
-            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-          </cdr:spPr>
-          <cdr:style>
-            <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-              <a:schemeClr val="dk1"/>
-            </a:lnRef>
-            <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:fillRef>
-            <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-              <a:schemeClr val="dk1"/>
-            </a:effectRef>
-            <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </cdr:style>
-        </cdr:cxnSp>
-      </cdr:grpSp>
-      <cdr:sp macro="" textlink="">
-        <cdr:nvSpPr>
-          <cdr:cNvPr id="40" name="ZoneTexte 3">
-            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{09AC7539-153F-4E2E-B975-AEF34DA4CB40}"/>
-              </a:ext>
-            </a:extLst>
-          </cdr:cNvPr>
-          <cdr:cNvSpPr txBox="1"/>
-        </cdr:nvSpPr>
-        <cdr:spPr>
-          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:off x="285204" y="6296"/>
-            <a:ext cx="179213" cy="178768"/>
-          </a:xfrm>
-          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </cdr:spPr>
-        <cdr:txBody>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:lvl1pPr marL="0" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" indent="0">
-              <a:defRPr sz="1100">
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:r>
-              <a:rPr lang="fr-FR" sz="1400" b="1"/>
-              <a:t>*</a:t>
-            </a:r>
-          </a:p>
-        </cdr:txBody>
-      </cdr:sp>
-    </cdr:grpSp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2110,7 +2646,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2143,9 +2679,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2178,6 +2731,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2353,19 +2923,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1025" width="10.28515625"/>
+    <col min="1" max="1025" width="10.26171875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2379,7 +2949,7 @@
       </c>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>4</v>
       </c>
@@ -2399,7 +2969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>5</v>
       </c>
@@ -2419,7 +2989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>5</v>
       </c>
@@ -2439,7 +3009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -2459,7 +3029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2479,7 +3049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2499,7 +3069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -2519,7 +3089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -2539,7 +3109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -2559,7 +3129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -2579,7 +3149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>5</v>
       </c>
@@ -2599,7 +3169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>4</v>
       </c>
@@ -2619,7 +3189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2639,7 +3209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>5</v>
       </c>
@@ -2659,7 +3229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -2679,7 +3249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -2699,7 +3269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
         <v>4</v>
       </c>
@@ -2719,7 +3289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
         <v>4</v>
       </c>
@@ -2739,7 +3309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -2759,7 +3329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
         <v>5</v>
       </c>
@@ -2779,7 +3349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
         <v>5</v>
       </c>
@@ -2799,7 +3369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
         <v>5</v>
       </c>
@@ -2819,7 +3389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2">
         <v>4</v>
       </c>
@@ -2839,7 +3409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
         <v>5</v>
       </c>
@@ -2859,7 +3429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -2879,7 +3449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
         <v>5</v>
       </c>
@@ -2899,7 +3469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2">
         <v>5</v>
       </c>
@@ -2919,7 +3489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -2939,7 +3509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -2959,7 +3529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2">
         <v>5</v>
       </c>
@@ -2979,7 +3549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -2999,7 +3569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
         <v>4</v>
       </c>
@@ -3019,7 +3589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2">
         <v>5</v>
       </c>
@@ -3039,7 +3609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2">
         <v>5</v>
       </c>
@@ -3059,7 +3629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2">
         <v>5</v>
       </c>
@@ -3079,7 +3649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2">
         <v>5</v>
       </c>
@@ -3099,7 +3669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2">
         <v>5</v>
       </c>
@@ -3119,7 +3689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
         <v>4</v>
       </c>
@@ -3139,7 +3709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2">
         <v>5</v>
       </c>
@@ -3159,7 +3729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
         <v>5</v>
       </c>
@@ -3179,7 +3749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
         <v>5</v>
       </c>
@@ -3199,7 +3769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
         <v>5</v>
       </c>
@@ -3219,7 +3789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
         <v>5</v>
       </c>
@@ -3239,7 +3809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
         <v>5</v>
       </c>
@@ -3259,7 +3829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2">
         <v>3</v>
       </c>
@@ -3279,7 +3849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2">
         <v>4</v>
       </c>
@@ -3299,7 +3869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2">
         <v>5</v>
       </c>
@@ -3319,7 +3889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2">
         <v>4</v>
       </c>
@@ -3339,7 +3909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2">
         <v>5</v>
       </c>
@@ -3359,7 +3929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
         <v>3</v>
       </c>
@@ -3379,7 +3949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2">
         <v>4</v>
       </c>
@@ -3399,7 +3969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2">
         <v>5</v>
       </c>
@@ -3419,7 +3989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2">
         <v>5</v>
       </c>
@@ -3439,7 +4009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2">
         <v>4</v>
       </c>
@@ -3459,7 +4029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2">
         <v>5</v>
       </c>
@@ -3479,7 +4049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2">
         <v>5</v>
       </c>
@@ -3499,7 +4069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2">
         <v>5</v>
       </c>
@@ -3519,7 +4089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2">
         <v>5</v>
       </c>
@@ -3539,7 +4109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
         <v>4</v>
       </c>
@@ -3559,7 +4129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2">
         <v>5</v>
       </c>
@@ -3579,7 +4149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2">
         <v>4</v>
       </c>
@@ -3610,39 +4180,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A4:G13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1025" width="10.28515625"/>
+    <col min="1" max="1025" width="10.26171875"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>AVERAGE(satPerceptif!A2:A62)</f>
         <v>4.5081967213114753</v>
@@ -3668,10 +4238,10 @@
         <v>3.8360655737704916</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f>_xlfn.STDEV.S(satPerceptif!A2:A62)</f>
         <v>0.72164051114277472</v>
@@ -3697,10 +4267,10 @@
         <v>0.98624418661324253</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10">
         <v>0.4773</v>
       </c>
@@ -3711,6 +4281,39 @@
       <c r="D7" s="10"/>
       <c r="E7" s="3">
         <v>0.80869999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>4.5081967213114753</v>
+      </c>
+      <c r="B12">
+        <v>4.4262295081967213</v>
+      </c>
+      <c r="C12">
+        <v>4.5081967213114753</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>3.8852459016393444</v>
+      </c>
+      <c r="B13">
+        <v>3.8360655737704916</v>
+      </c>
+      <c r="C13">
+        <v>3.8360655737704916</v>
       </c>
     </row>
   </sheetData>
@@ -3720,43 +4323,44 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMK61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:G67"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125" style="4"/>
+    <col min="1" max="1025" width="8.578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
@@ -3768,7 +4372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4">
         <v>17</v>
       </c>
@@ -3803,7 +4407,7 @@
         <v>0.49374999105930306</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4">
         <v>19</v>
       </c>
@@ -3838,7 +4442,7 @@
         <v>0.38541667908430122</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>20</v>
       </c>
@@ -3873,7 +4477,7 @@
         <v>0.50416666269302346</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4">
         <v>21</v>
       </c>
@@ -3908,7 +4512,7 @@
         <v>0.45833334326744102</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>23</v>
       </c>
@@ -3943,7 +4547,7 @@
         <v>0.58333332836627949</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4">
         <v>24</v>
       </c>
@@ -3978,7 +4582,7 @@
         <v>0.59166666865348805</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>25</v>
       </c>
@@ -4013,7 +4617,7 @@
         <v>0.51874999701976798</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4">
         <v>26</v>
       </c>
@@ -4048,7 +4652,7 @@
         <v>0.51041665673255898</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4">
         <v>27</v>
       </c>
@@ -4083,7 +4687,7 @@
         <v>0.62291665375232652</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4">
         <v>28</v>
       </c>
@@ -4118,7 +4722,7 @@
         <v>0.63541665673255898</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4">
         <v>29</v>
       </c>
@@ -4153,7 +4757,7 @@
         <v>0.48333333432674408</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4">
         <v>30</v>
       </c>
@@ -4188,7 +4792,7 @@
         <v>0.55000001192092907</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4">
         <v>31</v>
       </c>
@@ -4223,7 +4827,7 @@
         <v>0.53541666269302346</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4">
         <v>32</v>
       </c>
@@ -4258,7 +4862,7 @@
         <v>0.55624999105930295</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4">
         <v>33</v>
       </c>
@@ -4293,7 +4897,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4">
         <v>34</v>
       </c>
@@ -4328,7 +4932,7 @@
         <v>0.51458333432674397</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
         <v>35</v>
       </c>
@@ -4363,7 +4967,7 @@
         <v>0.59166665375232652</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4">
         <v>36</v>
       </c>
@@ -4398,7 +5002,7 @@
         <v>0.47499998658895498</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
         <v>37</v>
       </c>
@@ -4433,7 +5037,7 @@
         <v>0.47916666418314002</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4">
         <v>38</v>
       </c>
@@ -4468,7 +5072,7 @@
         <v>0.55208334326744102</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
         <v>39</v>
       </c>
@@ -4503,7 +5107,7 @@
         <v>0.51666666567325548</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4">
         <v>40</v>
       </c>
@@ -4538,7 +5142,7 @@
         <v>0.46666665375232697</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4">
         <v>41</v>
       </c>
@@ -4573,7 +5177,7 @@
         <v>0.55208334326744057</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4">
         <v>42</v>
       </c>
@@ -4608,7 +5212,7 @@
         <v>0.69374999403953552</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4">
         <v>44</v>
       </c>
@@ -4643,7 +5247,7 @@
         <v>0.52499997615814198</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4">
         <v>45</v>
       </c>
@@ -4678,7 +5282,7 @@
         <v>0.53541666269302346</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4">
         <v>46</v>
       </c>
@@ -4713,7 +5317,7 @@
         <v>0.43333330750465399</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4">
         <v>47</v>
       </c>
@@ -4748,7 +5352,7 @@
         <v>0.61249999701976798</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4">
         <v>48</v>
       </c>
@@ -4783,7 +5387,7 @@
         <v>0.62291666120290756</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4">
         <v>49</v>
       </c>
@@ -4818,7 +5422,7 @@
         <v>0.69791665673255898</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4">
         <v>50</v>
       </c>
@@ -4853,7 +5457,7 @@
         <v>0.55208332836627949</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4">
         <v>51</v>
       </c>
@@ -4888,7 +5492,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4">
         <v>52</v>
       </c>
@@ -4923,7 +5527,7 @@
         <v>0.47291665524244297</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4">
         <v>53</v>
       </c>
@@ -4958,7 +5562,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4">
         <v>54</v>
       </c>
@@ -4993,7 +5597,7 @@
         <v>0.52083332836627949</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4">
         <v>55</v>
       </c>
@@ -5028,7 +5632,7 @@
         <v>0.422916680574417</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4">
         <v>56</v>
       </c>
@@ -5063,7 +5667,7 @@
         <v>0.58958332240581501</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4">
         <v>57</v>
       </c>
@@ -5098,7 +5702,7 @@
         <v>0.633333340287209</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4">
         <v>58</v>
       </c>
@@ -5133,7 +5737,7 @@
         <v>0.55833330750465393</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4">
         <v>59</v>
       </c>
@@ -5168,7 +5772,7 @@
         <v>0.63333332538604747</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4">
         <v>60</v>
       </c>
@@ -5203,7 +5807,7 @@
         <v>0.45833332836627999</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4">
         <v>61</v>
       </c>
@@ -5238,7 +5842,7 @@
         <v>0.50416666269302346</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4">
         <v>62</v>
       </c>
@@ -5273,7 +5877,7 @@
         <v>0.54166665673255898</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4">
         <v>63</v>
       </c>
@@ -5308,7 +5912,7 @@
         <v>0.5104166492819785</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4">
         <v>64</v>
       </c>
@@ -5343,7 +5947,7 @@
         <v>0.60416665673255898</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4">
         <v>65</v>
       </c>
@@ -5378,7 +5982,7 @@
         <v>0.53749999403953552</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4">
         <v>66</v>
       </c>
@@ -5413,7 +6017,7 @@
         <v>0.55416667461395253</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4">
         <v>67</v>
       </c>
@@ -5448,7 +6052,7 @@
         <v>0.61458334326744057</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4">
         <v>68</v>
       </c>
@@ -5483,7 +6087,7 @@
         <v>0.50625000894069694</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4">
         <v>69</v>
       </c>
@@ -5518,7 +6122,7 @@
         <v>0.41041666269302352</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4">
         <v>70</v>
       </c>
@@ -5553,7 +6157,7 @@
         <v>0.58333332836627949</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4">
         <v>71</v>
       </c>
@@ -5588,7 +6192,7 @@
         <v>0.52083332836627949</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4">
         <v>72</v>
       </c>
@@ -5623,7 +6227,7 @@
         <v>0.46874997764825854</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4">
         <v>73</v>
       </c>
@@ -5658,7 +6262,7 @@
         <v>0.52499999850988388</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4">
         <v>74</v>
       </c>
@@ -5693,7 +6297,7 @@
         <v>0.61249999701976754</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="4">
         <v>75</v>
       </c>
@@ -5728,7 +6332,7 @@
         <v>0.46249999105930351</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4">
         <v>76</v>
       </c>
@@ -5763,7 +6367,7 @@
         <v>0.33541666716337204</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="4">
         <v>77</v>
       </c>
@@ -5798,7 +6402,7 @@
         <v>0.54583331197500251</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4">
         <v>78</v>
       </c>
@@ -5833,7 +6437,7 @@
         <v>0.52500000596046448</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="4">
         <v>79</v>
       </c>
@@ -5866,122 +6470,6 @@
       <c r="L61" s="4">
         <f>AVERAGE(F61:G61)</f>
         <v>0.54374998807907104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="4">
-        <f>AVERAGE(B2:'restaurantsSat'!B61)</f>
-        <v>0.71458332414428394</v>
-      </c>
-      <c r="C63" s="4">
-        <f>AVERAGE(C2:'restaurantsSat'!C61)</f>
-        <v>0.52819444090127943</v>
-      </c>
-      <c r="D63" s="4">
-        <f>AVERAGE(D2:'restaurantsSat'!D61)</f>
-        <v>0.68034721066554371</v>
-      </c>
-      <c r="E63" s="4">
-        <f>AVERAGE(E2:'restaurantsSat'!E61)</f>
-        <v>0.32618055393298467</v>
-      </c>
-      <c r="F63" s="4">
-        <f>AVERAGE(F2:'restaurantsSat'!F61)</f>
-        <v>0.72868054732680321</v>
-      </c>
-      <c r="G63" s="4">
-        <f>AVERAGE(G2:'restaurantsSat'!G61)</f>
-        <v>0.33826388791203493</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="4">
-        <f>_xlfn.STDEV.S(B2:B61)</f>
-        <v>0.19785142664511576</v>
-      </c>
-      <c r="C64" s="4">
-        <f t="shared" ref="C64:G64" si="3">_xlfn.STDEV.S(C2:C61)</f>
-        <v>0.24145271750739275</v>
-      </c>
-      <c r="D64" s="4">
-        <f t="shared" si="3"/>
-        <v>0.17701305506883414</v>
-      </c>
-      <c r="E64" s="4">
-        <f t="shared" si="3"/>
-        <v>0.18909334115130935</v>
-      </c>
-      <c r="F64" s="4">
-        <f t="shared" si="3"/>
-        <v>0.18457478037627015</v>
-      </c>
-      <c r="G64" s="4">
-        <f t="shared" si="3"/>
-        <v>0.16378240842538308</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B66" s="4">
-        <f>MIN(B2:B61)</f>
-        <v>0.1875</v>
-      </c>
-      <c r="C66" s="4">
-        <f t="shared" ref="C66:G66" si="4">MIN(C2:C61)</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="D66" s="4">
-        <f t="shared" si="4"/>
-        <v>0.29166665673255898</v>
-      </c>
-      <c r="E66" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F66" s="4">
-        <f t="shared" si="4"/>
-        <v>4.1666671633720398E-2</v>
-      </c>
-      <c r="G66" s="4">
-        <f t="shared" si="4"/>
-        <v>4.9999997019767803E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" s="4">
-        <f>MAX(B2:B61)</f>
-        <v>1</v>
-      </c>
-      <c r="C67" s="4">
-        <f t="shared" ref="C67:G67" si="5">MAX(C2:C61)</f>
-        <v>1</v>
-      </c>
-      <c r="D67" s="4">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="E67" s="4">
-        <f t="shared" si="5"/>
-        <v>0.875</v>
-      </c>
-      <c r="F67" s="4">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G67" s="4">
-        <f t="shared" si="5"/>
-        <v>0.77083331346511796</v>
       </c>
     </row>
   </sheetData>
@@ -5995,37 +6483,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" style="4" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="4" customWidth="1"/>
-    <col min="5" max="1025" width="8.5703125" style="4"/>
+    <col min="3" max="3" width="13.83984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.41796875" style="4" customWidth="1"/>
+    <col min="5" max="1025" width="8.578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6">
         <v>0.62138888252278168</v>
@@ -6037,9 +6525,9 @@
         <v>0.5334722176194191</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6">
         <v>6.4869018305032389E-2</v>
@@ -6051,29 +6539,29 @@
         <v>7.1606845378041767E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="B6" s="5">
         <v>8.8909000000000002</v>
@@ -6085,9 +6573,9 @@
         <v>2.2964000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="7">
         <v>1.737E-12</v>
@@ -6099,24 +6587,24 @@
         <v>2.5219999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0.55000000000000004</v>
       </c>
@@ -6136,7 +6624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>0.65</v>
       </c>
@@ -6156,7 +6644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0.65</v>
       </c>
@@ -6176,7 +6664,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>0.63</v>
       </c>

</xml_diff>